<commit_message>
added tabs for RES figures
</commit_message>
<xml_diff>
--- a/dashboard/Data/economic_parameters.xlsx
+++ b/dashboard/Data/economic_parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardumi\repository\unescap\dashboard\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camilorg\Box Sync\UNESCAP\unescap_model\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>scenario</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>$1967 Billion</t>
+  </si>
+  <si>
+    <t>$1552 Billion</t>
+  </si>
+  <si>
+    <t>$1414 Billion</t>
   </si>
 </sst>
 </file>
@@ -377,12 +386,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -400,8 +410,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1967</v>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -411,8 +421,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>1552</v>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -422,8 +432,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>1414</v>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
all scenarios and descriptions updated
</commit_message>
<xml_diff>
--- a/dashboard/Data/economic_parameters.xlsx
+++ b/dashboard/Data/economic_parameters.xlsx
@@ -50,13 +50,13 @@
     <t>NA</t>
   </si>
   <si>
-    <t>$1812 Billion</t>
-  </si>
-  <si>
-    <t>$1421 Billion</t>
-  </si>
-  <si>
-    <t>$1467 Billion</t>
+    <t>$1023 Billion</t>
+  </si>
+  <si>
+    <t>$1197 Billion</t>
+  </si>
+  <si>
+    <t>$994 Billion</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -411,7 +411,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -422,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -433,7 +433,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>

</xml_diff>